<commit_message>
adding mutation condense to clinscore panel design
</commit_message>
<xml_diff>
--- a/testdata/test_mutations_hg19.xlsx
+++ b/testdata/test_mutations_hg19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinszyska/Sites/Bio/pyseq/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC60493-9A14-144B-9557-6D5DE7E34C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E99BDE-C263-5943-B5B1-E3F9628EBD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23280" yWindow="1080" windowWidth="28160" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2367,7 +2367,7 @@
   <dimension ref="A1:AH20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3789,18 +3789,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3822,6 +3822,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69085103-7E58-4853-8232-47AD2E4A8907}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3172CC7D-8658-414D-A4FD-4A05361F4F41}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3835,12 +3843,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69085103-7E58-4853-8232-47AD2E4A8907}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>